<commit_message>
added new input files
</commit_message>
<xml_diff>
--- a/Results/2024-03-13/2024-03-13_PE_MP_Emissions_freeMP_5000.0_nm_/Compartment_mass_flows/Agricultural_Soil_Surface_mass_flows.xlsx
+++ b/Results/2024-03-13/2024-03-13_PE_MP_Emissions_freeMP_5000.0_nm_/Compartment_mass_flows/Agricultural_Soil_Surface_mass_flows.xlsx
@@ -454,13 +454,13 @@
         <v>8</v>
       </c>
       <c r="C2">
-        <v>0.00104795803730061</v>
+        <v>3.778367079667894E-31</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
       <c r="E2">
-        <v>0.003063197658106027</v>
+        <v>1.104422579716672E-30</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -469,7 +469,7 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>3.056666319815822E-18</v>
+        <v>1.102067734130922E-45</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -480,13 +480,13 @@
         <v>8</v>
       </c>
       <c r="C3">
-        <v>0.000233124482236184</v>
+        <v>5.716201930652014E-32</v>
       </c>
       <c r="D3">
-        <v>2.303613249533904E-05</v>
+        <v>5.64844943703533E-33</v>
       </c>
       <c r="E3">
-        <v>0.0006814264909618852</v>
+        <v>1.670854723566727E-31</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -495,7 +495,7 @@
         <v>0</v>
       </c>
       <c r="H3">
-        <v>6.799735560131391E-19</v>
+        <v>1.6672921335378E-46</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -506,13 +506,13 @@
         <v>8</v>
       </c>
       <c r="C4">
-        <v>0.0001218154176059246</v>
+        <v>2.488138434518548E-32</v>
       </c>
       <c r="D4">
-        <v>0.0001203715745780038</v>
+        <v>2.458647246935026E-32</v>
       </c>
       <c r="E4">
-        <v>0.0003560683621386628</v>
+        <v>7.272867380542371E-32</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -521,7 +521,7 @@
         <v>0</v>
       </c>
       <c r="H4">
-        <v>3.553091545434844E-19</v>
+        <v>7.257360200626503E-47</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -532,13 +532,13 @@
         <v>8</v>
       </c>
       <c r="C5">
-        <v>2.02213914023472E-05</v>
+        <v>4.129709236116288E-33</v>
       </c>
       <c r="D5">
-        <v>0.0001998171307948015</v>
+        <v>4.080760983053643E-32</v>
       </c>
       <c r="E5">
-        <v>5.91074418846668E-05</v>
+        <v>1.207120439031618E-32</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -547,7 +547,7 @@
         <v>0</v>
       </c>
       <c r="H5">
-        <v>5.89814132239319E-20</v>
+        <v>1.204546621464386E-47</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -558,13 +558,13 @@
         <v>8</v>
       </c>
       <c r="C6">
-        <v>5.649885748665548E-05</v>
+        <v>1.137687157862589E-32</v>
       </c>
       <c r="D6">
-        <v>0.005582919281636311</v>
+        <v>1.124202479953024E-30</v>
       </c>
       <c r="E6">
-        <v>0.0001651470400328104</v>
+        <v>3.325477274451507E-32</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -573,7 +573,7 @@
         <v>0</v>
       </c>
       <c r="H6">
-        <v>1.64794914147879E-19</v>
+        <v>3.318386704569947E-47</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -584,13 +584,13 @@
         <v>9</v>
       </c>
       <c r="C7">
-        <v>6.09242939038771E-24</v>
+        <v>6.868515494336825E-24</v>
       </c>
       <c r="D7">
         <v>0</v>
       </c>
       <c r="E7">
-        <v>1.780826595775096E-22</v>
+        <v>2.007677772204751E-22</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -599,7 +599,7 @@
         <v>0</v>
       </c>
       <c r="H7">
-        <v>1.777029524142313E-37</v>
+        <v>2.00339700936423E-37</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -610,13 +610,13 @@
         <v>9</v>
       </c>
       <c r="C8">
-        <v>1.798987049742852E-24</v>
+        <v>1.51096979741406E-24</v>
       </c>
       <c r="D8">
-        <v>1.778256532170809E-26</v>
+        <v>1.493558229086986E-26</v>
       </c>
       <c r="E8">
-        <v>5.258467153828056E-23</v>
+        <v>4.416588241290444E-23</v>
       </c>
       <c r="F8">
         <v>0</v>
@@ -625,7 +625,7 @@
         <v>0</v>
       </c>
       <c r="H8">
-        <v>5.247255070344414E-38</v>
+        <v>4.407171208793022E-38</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -636,13 +636,13 @@
         <v>9</v>
       </c>
       <c r="C9">
-        <v>1.090436932400156E-24</v>
+        <v>1.004318580794982E-24</v>
       </c>
       <c r="D9">
-        <v>1.077512656962345E-25</v>
+        <v>9.924150129866769E-26</v>
       </c>
       <c r="E9">
-        <v>3.187364129812312E-23</v>
+        <v>2.935638847341629E-23</v>
       </c>
       <c r="F9">
         <v>0</v>
@@ -651,7 +651,7 @@
         <v>0</v>
       </c>
       <c r="H9">
-        <v>3.18056804424768E-38</v>
+        <v>2.929379489458171E-38</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -662,13 +662,13 @@
         <v>9</v>
       </c>
       <c r="C10">
-        <v>4.047727475832182E-25</v>
+        <v>4.86279766474278E-25</v>
       </c>
       <c r="D10">
-        <v>3.999750930273725E-25</v>
+        <v>4.805160327472162E-25</v>
       </c>
       <c r="E10">
-        <v>1.183157042867726E-23</v>
+        <v>1.421403328023779E-23</v>
       </c>
       <c r="F10">
         <v>0</v>
@@ -677,7 +677,7 @@
         <v>0</v>
       </c>
       <c r="H10">
-        <v>1.180634319961825E-38</v>
+        <v>1.418372617303046E-38</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -688,13 +688,13 @@
         <v>9</v>
       </c>
       <c r="C11">
-        <v>2.055315928493427E-23</v>
+        <v>2.910959712343323E-23</v>
       </c>
       <c r="D11">
-        <v>2.030954861300378E-22</v>
+        <v>2.87645694604567E-22</v>
       </c>
       <c r="E11">
-        <v>6.007720457057862E-22</v>
+        <v>8.508780558293708E-22</v>
       </c>
       <c r="F11">
         <v>0</v>
@@ -703,7 +703,7 @@
         <v>0</v>
       </c>
       <c r="H11">
-        <v>5.994910818556673E-37</v>
+        <v>8.490638169043614E-37</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -714,13 +714,13 @@
         <v>10</v>
       </c>
       <c r="C12">
-        <v>5.005107295494086E-29</v>
+        <v>9.35041305906861E-30</v>
       </c>
       <c r="D12">
         <v>0</v>
       </c>
       <c r="E12">
-        <v>7.315003273231707E-28</v>
+        <v>1.366570147152127E-28</v>
       </c>
       <c r="F12">
         <v>0</v>
@@ -729,7 +729,7 @@
         <v>0</v>
       </c>
       <c r="H12">
-        <v>7.299406251327161E-43</v>
+        <v>1.363656351529201E-43</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -740,13 +740,13 @@
         <v>10</v>
       </c>
       <c r="C13">
-        <v>1.615303704071233E-30</v>
+        <v>2.217554674555373E-30</v>
       </c>
       <c r="D13">
-        <v>1.197118481195107E-30</v>
+        <v>1.643452978706083E-30</v>
       </c>
       <c r="E13">
-        <v>2.360778937382989E-29</v>
+        <v>3.240973418800907E-29</v>
       </c>
       <c r="F13">
         <v>0</v>
@@ -755,7 +755,7 @@
         <v>0</v>
       </c>
       <c r="H13">
-        <v>2.35574529359326E-44</v>
+        <v>3.234063027716043E-44</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -766,13 +766,13 @@
         <v>10</v>
       </c>
       <c r="C14">
-        <v>1.030466633274008E-30</v>
+        <v>1.41249715287088E-30</v>
       </c>
       <c r="D14">
-        <v>3.054758427998544E-30</v>
+        <v>4.187265693938215E-30</v>
       </c>
       <c r="E14">
-        <v>1.506035005911161E-29</v>
+        <v>2.064375584112423E-29</v>
       </c>
       <c r="F14">
         <v>0</v>
@@ -781,7 +781,7 @@
         <v>0</v>
       </c>
       <c r="H14">
-        <v>1.502823843851649E-44</v>
+        <v>2.059973930414955E-44</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -792,13 +792,13 @@
         <v>10</v>
       </c>
       <c r="C15">
-        <v>1.542284132906619E-30</v>
+        <v>2.063643899925368E-30</v>
       </c>
       <c r="D15">
-        <v>3.886209903407255E-29</v>
+        <v>5.19991951540197E-29</v>
       </c>
       <c r="E15">
-        <v>2.254060265725341E-29</v>
+        <v>3.016031623603492E-29</v>
       </c>
       <c r="F15">
         <v>0</v>
@@ -807,7 +807,7 @@
         <v>0</v>
       </c>
       <c r="H15">
-        <v>2.24925416707774E-44</v>
+        <v>3.009600852551033E-44</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -818,13 +818,13 @@
         <v>10</v>
       </c>
       <c r="C16">
-        <v>4.594586973626238E-31</v>
+        <v>6.400616063262757E-31</v>
       </c>
       <c r="D16">
-        <v>1.137302229018351E-28</v>
+        <v>1.584350227261922E-28</v>
       </c>
       <c r="E16">
-        <v>6.715024627240462E-30</v>
+        <v>9.354550200275888E-30</v>
       </c>
       <c r="F16">
         <v>0</v>
@@ -833,7 +833,7 @@
         <v>0</v>
       </c>
       <c r="H16">
-        <v>6.700706877502209E-45</v>
+        <v>9.334604464241184E-45</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -844,13 +844,13 @@
         <v>11</v>
       </c>
       <c r="C17">
-        <v>2.130762217830989E-22</v>
+        <v>2.962438639842334E-22</v>
       </c>
       <c r="D17">
         <v>0</v>
       </c>
       <c r="E17">
-        <v>1.245650227074582E-20</v>
+        <v>1.731850852964027E-20</v>
       </c>
       <c r="F17">
         <v>0</v>
@@ -859,7 +859,7 @@
         <v>0</v>
       </c>
       <c r="H17">
-        <v>1.24299425644116E-35</v>
+        <v>1.728158207222099E-35</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -870,13 +870,13 @@
         <v>11</v>
       </c>
       <c r="C18">
-        <v>4.681476829039305E-23</v>
+        <v>6.502088497000151E-23</v>
       </c>
       <c r="D18">
-        <v>1.38781372320813E-24</v>
+        <v>1.927530131021133E-24</v>
       </c>
       <c r="E18">
-        <v>2.736805930918639E-21</v>
+        <v>3.801141180826823E-21</v>
       </c>
       <c r="F18">
         <v>0</v>
@@ -885,7 +885,7 @@
         <v>0</v>
       </c>
       <c r="H18">
-        <v>2.730970523816467E-36</v>
+        <v>3.793036402189665E-36</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -896,13 +896,13 @@
         <v>11</v>
       </c>
       <c r="C19">
-        <v>3.222210768445213E-23</v>
+        <v>4.469393191148656E-23</v>
       </c>
       <c r="D19">
-        <v>3.820823336768592E-24</v>
+        <v>5.299703536828331E-24</v>
       </c>
       <c r="E19">
-        <v>1.883714448194853E-21</v>
+        <v>2.612821175845304E-21</v>
       </c>
       <c r="F19">
         <v>0</v>
@@ -911,7 +911,7 @@
         <v>0</v>
       </c>
       <c r="H19">
-        <v>1.87969799947802E-36</v>
+        <v>2.607250128562052E-36</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -922,13 +922,13 @@
         <v>11</v>
       </c>
       <c r="C20">
-        <v>9.612188150888201E-22</v>
+        <v>1.28176280499315E-21</v>
       </c>
       <c r="D20">
-        <v>9.688222811896314E-22</v>
+        <v>1.291901849177533E-21</v>
       </c>
       <c r="E20">
-        <v>5.619315122372429E-20</v>
+        <v>7.493225268095654E-20</v>
       </c>
       <c r="F20">
         <v>0</v>
@@ -937,7 +937,7 @@
         <v>0</v>
       </c>
       <c r="H20">
-        <v>5.607333640235174E-35</v>
+        <v>7.477248241937667E-35</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -948,13 +948,13 @@
         <v>11</v>
       </c>
       <c r="C21">
-        <v>1.743161607210938E-21</v>
+        <v>2.428359338504686E-21</v>
       </c>
       <c r="D21">
-        <v>1.725945416030462E-20</v>
+        <v>2.404375848704516E-20</v>
       </c>
       <c r="E21">
-        <v>1.019057703238396E-19</v>
+        <v>1.419626430445265E-19</v>
       </c>
       <c r="F21">
         <v>0</v>
@@ -963,7 +963,7 @@
         <v>0</v>
       </c>
       <c r="H21">
-        <v>1.016884872314647E-34</v>
+        <v>1.41659950841873E-34</v>
       </c>
     </row>
   </sheetData>
@@ -1001,7 +1001,7 @@
         <v>8</v>
       </c>
       <c r="C2">
-        <v>8.868925726386067E-19</v>
+        <v>6.528913001463132E-31</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -1015,7 +1015,7 @@
         <v>8</v>
       </c>
       <c r="C3">
-        <v>1.97294204655824E-19</v>
+        <v>4.081081090649225E-32</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -1029,7 +1029,7 @@
         <v>8</v>
       </c>
       <c r="C4">
-        <v>1.030928868399824E-19</v>
+        <v>1.614760658549803E-33</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -1043,7 +1043,7 @@
         <v>8</v>
       </c>
       <c r="C5">
-        <v>1.711344636467282E-20</v>
+        <v>7.983994593176807E-34</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -1057,7 +1057,7 @@
         <v>8</v>
       </c>
       <c r="C6">
-        <v>0.005804565179155776</v>
+        <v>1.168834124276165E-30</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -1071,7 +1071,7 @@
         <v>9</v>
       </c>
       <c r="C7">
-        <v>4.169660542288476E-23</v>
+        <v>5.931440539026776E-24</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -1085,7 +1085,7 @@
         <v>9</v>
       </c>
       <c r="C8">
-        <v>2.380324758238592E-23</v>
+        <v>2.399209644725598E-24</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -1099,7 +1099,7 @@
         <v>9</v>
       </c>
       <c r="C9">
-        <v>1.268228586461028E-23</v>
+        <v>1.599275888503827E-24</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -1113,7 +1113,7 @@
         <v>9</v>
       </c>
       <c r="C10">
-        <v>2.48154396278597E-24</v>
+        <v>7.985443492309426E-25</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -1127,7 +1127,7 @@
         <v>9</v>
       </c>
       <c r="C11">
-        <v>8.244206911207592E-22</v>
+        <v>1.167633347557372E-21</v>
       </c>
       <c r="D11">
         <v>0</v>
@@ -1141,7 +1141,7 @@
         <v>10</v>
       </c>
       <c r="C12">
-        <v>6.758984871311899E-28</v>
+        <v>1.663089478598818E-31</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -1155,7 +1155,7 @@
         <v>10</v>
       </c>
       <c r="C13">
-        <v>6.087910300720303E-32</v>
+        <v>1.201655456867828E-32</v>
       </c>
       <c r="D13">
         <v>0</v>
@@ -1169,7 +1169,7 @@
         <v>10</v>
       </c>
       <c r="C14">
-        <v>1.33023386149462E-34</v>
+        <v>1.773845101826831E-34</v>
       </c>
       <c r="D14">
         <v>0</v>
@@ -1183,7 +1183,7 @@
         <v>10</v>
       </c>
       <c r="C15">
-        <v>5.725847467914086E-29</v>
+        <v>7.630140415367042E-29</v>
       </c>
       <c r="D15">
         <v>0</v>
@@ -1197,7 +1197,7 @@
         <v>10</v>
       </c>
       <c r="C16">
-        <v>1.209047062264382E-28</v>
+        <v>1.684296345327944E-28</v>
       </c>
       <c r="D16">
         <v>0</v>
@@ -1211,7 +1211,7 @@
         <v>11</v>
       </c>
       <c r="C17">
-        <v>3.368986210329239E-24</v>
+        <v>4.402961286951134E-24</v>
       </c>
       <c r="D17">
         <v>0</v>
@@ -1225,7 +1225,7 @@
         <v>11</v>
       </c>
       <c r="C18">
-        <v>4.155209802399598E-25</v>
+        <v>4.956012671549488E-25</v>
       </c>
       <c r="D18">
         <v>0</v>
@@ -1239,7 +1239,7 @@
         <v>11</v>
       </c>
       <c r="C19">
-        <v>4.750694768795333E-26</v>
+        <v>5.859275359892083E-26</v>
       </c>
       <c r="D19">
         <v>0</v>
@@ -1253,7 +1253,7 @@
         <v>11</v>
       </c>
       <c r="C20">
-        <v>5.726021961198758E-20</v>
+        <v>7.630372941077504E-20</v>
       </c>
       <c r="D20">
         <v>0</v>
@@ -1267,7 +1267,7 @@
         <v>11</v>
       </c>
       <c r="C21">
-        <v>1.209083860913553E-19</v>
+        <v>1.684347608700765E-19</v>
       </c>
       <c r="D21">
         <v>0</v>

</xml_diff>